<commit_message>
early withdrawal in scripts WIP complete
</commit_message>
<xml_diff>
--- a/data/EARLY_WITHDRAWAL_DATA.xlsx
+++ b/data/EARLY_WITHDRAWAL_DATA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adevr\riskactive_main\FRTB\From_Sait\Early Withdrawal Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adevr\ra_frtb\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C70A1AD-C79F-4A46-9493-E16A90EBCA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D1BD2F-242B-4A9D-BAEF-85A652F6EFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="19">
   <si>
     <t>REPORT_DATE</t>
   </si>
@@ -553,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,6 +2031,1419 @@
         <v>18</v>
       </c>
     </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>44805</v>
+      </c>
+      <c r="B34" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C34" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D34" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E34" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H34" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I34" s="8">
+        <f>A34</f>
+        <v>44805</v>
+      </c>
+      <c r="J34" s="8">
+        <f>A34</f>
+        <v>44805</v>
+      </c>
+      <c r="K34" s="8">
+        <f>J34+90</f>
+        <v>44895</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>45901</v>
+      </c>
+      <c r="B35" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C35" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D35" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E35" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="10">
+        <v>47</v>
+      </c>
+      <c r="H35" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I35" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J35" s="8">
+        <f t="shared" ref="J35:J37" si="12">A35</f>
+        <v>45901</v>
+      </c>
+      <c r="K35" s="8">
+        <f t="shared" ref="K35:K41" si="13">J35+90</f>
+        <v>45991</v>
+      </c>
+      <c r="L35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M35" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <f>A34+1</f>
+        <v>44806</v>
+      </c>
+      <c r="B36" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C36" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D36" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E36" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H36" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I36" s="8">
+        <v>45908</v>
+      </c>
+      <c r="J36" s="8">
+        <f t="shared" si="12"/>
+        <v>44806</v>
+      </c>
+      <c r="K36" s="8">
+        <f t="shared" si="13"/>
+        <v>44896</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>44806</v>
+      </c>
+      <c r="B37" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C37" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D37" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E37" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="10">
+        <v>47</v>
+      </c>
+      <c r="H37" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I37" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J37" s="8">
+        <f t="shared" si="12"/>
+        <v>44806</v>
+      </c>
+      <c r="K37" s="8">
+        <f t="shared" si="13"/>
+        <v>44896</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <f t="shared" ref="A38:A65" si="14">A36+1</f>
+        <v>44807</v>
+      </c>
+      <c r="B38" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C38" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D38" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H38" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I38" s="8">
+        <f>A38</f>
+        <v>44807</v>
+      </c>
+      <c r="J38" s="8">
+        <f>A38</f>
+        <v>44807</v>
+      </c>
+      <c r="K38" s="8">
+        <f>J38+90</f>
+        <v>44897</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M38" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <f t="shared" si="14"/>
+        <v>44807</v>
+      </c>
+      <c r="B39" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C39" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D39" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E39" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10">
+        <v>47</v>
+      </c>
+      <c r="H39" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I39" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J39" s="8">
+        <f t="shared" ref="J39:J41" si="15">A39</f>
+        <v>44807</v>
+      </c>
+      <c r="K39" s="8">
+        <f t="shared" ref="K39:K45" si="16">J39+90</f>
+        <v>44897</v>
+      </c>
+      <c r="L39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M39" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <f t="shared" si="14"/>
+        <v>44808</v>
+      </c>
+      <c r="B40" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C40" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D40" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H40" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I40" s="8">
+        <v>45908</v>
+      </c>
+      <c r="J40" s="8">
+        <f t="shared" si="15"/>
+        <v>44808</v>
+      </c>
+      <c r="K40" s="8">
+        <f t="shared" si="16"/>
+        <v>44898</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M40" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <f t="shared" si="14"/>
+        <v>44808</v>
+      </c>
+      <c r="B41" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C41" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D41" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E41" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="10">
+        <v>47</v>
+      </c>
+      <c r="H41" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I41" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J41" s="8">
+        <f t="shared" si="15"/>
+        <v>44808</v>
+      </c>
+      <c r="K41" s="8">
+        <f t="shared" si="16"/>
+        <v>44898</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <f t="shared" si="14"/>
+        <v>44809</v>
+      </c>
+      <c r="B42" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C42" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D42" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H42" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I42" s="8">
+        <f>A42</f>
+        <v>44809</v>
+      </c>
+      <c r="J42" s="8">
+        <f>A42</f>
+        <v>44809</v>
+      </c>
+      <c r="K42" s="8">
+        <f>J42+180</f>
+        <v>44989</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M42" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <f t="shared" si="14"/>
+        <v>44809</v>
+      </c>
+      <c r="B43" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C43" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D43" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E43" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="10">
+        <v>47</v>
+      </c>
+      <c r="H43" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I43" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J43" s="8">
+        <f t="shared" ref="J43:J45" si="17">A43</f>
+        <v>44809</v>
+      </c>
+      <c r="K43" s="8">
+        <f t="shared" ref="K43:K49" si="18">J43+180</f>
+        <v>44989</v>
+      </c>
+      <c r="L43" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M43" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <f t="shared" si="14"/>
+        <v>44810</v>
+      </c>
+      <c r="B44" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C44" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D44" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H44" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I44" s="8">
+        <v>45908</v>
+      </c>
+      <c r="J44" s="8">
+        <f t="shared" si="17"/>
+        <v>44810</v>
+      </c>
+      <c r="K44" s="8">
+        <f t="shared" si="18"/>
+        <v>44990</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M44" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <f t="shared" si="14"/>
+        <v>44810</v>
+      </c>
+      <c r="B45" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C45" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D45" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E45" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="10">
+        <v>47</v>
+      </c>
+      <c r="H45" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I45" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J45" s="8">
+        <f t="shared" si="17"/>
+        <v>44810</v>
+      </c>
+      <c r="K45" s="8">
+        <f t="shared" si="18"/>
+        <v>44990</v>
+      </c>
+      <c r="L45" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M45" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <f t="shared" si="14"/>
+        <v>44811</v>
+      </c>
+      <c r="B46" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C46" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D46" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H46" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I46" s="8">
+        <f>A46</f>
+        <v>44811</v>
+      </c>
+      <c r="J46" s="8">
+        <f>A46</f>
+        <v>44811</v>
+      </c>
+      <c r="K46" s="8">
+        <f t="shared" si="18"/>
+        <v>44991</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M46" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <f t="shared" si="14"/>
+        <v>44811</v>
+      </c>
+      <c r="B47" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C47" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D47" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E47" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="10">
+        <v>47</v>
+      </c>
+      <c r="H47" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I47" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J47" s="8">
+        <f t="shared" ref="J47:J49" si="19">A47</f>
+        <v>44811</v>
+      </c>
+      <c r="K47" s="8">
+        <f t="shared" si="18"/>
+        <v>44991</v>
+      </c>
+      <c r="L47" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M47" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <f t="shared" si="14"/>
+        <v>44812</v>
+      </c>
+      <c r="B48" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C48" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D48" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H48" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I48" s="8">
+        <v>45908</v>
+      </c>
+      <c r="J48" s="8">
+        <f t="shared" si="19"/>
+        <v>44812</v>
+      </c>
+      <c r="K48" s="8">
+        <f t="shared" si="18"/>
+        <v>44992</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M48" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <f t="shared" si="14"/>
+        <v>44812</v>
+      </c>
+      <c r="B49" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C49" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D49" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E49" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="10">
+        <v>47</v>
+      </c>
+      <c r="H49" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I49" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J49" s="8">
+        <f t="shared" si="19"/>
+        <v>44812</v>
+      </c>
+      <c r="K49" s="8">
+        <f t="shared" si="18"/>
+        <v>44992</v>
+      </c>
+      <c r="L49" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M49" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <f t="shared" si="14"/>
+        <v>44813</v>
+      </c>
+      <c r="B50" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C50" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D50" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E50" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H50" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I50" s="8">
+        <f>A50</f>
+        <v>44813</v>
+      </c>
+      <c r="J50" s="8">
+        <f>A50</f>
+        <v>44813</v>
+      </c>
+      <c r="K50" s="8">
+        <f>J50+360</f>
+        <v>45173</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M50" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <f t="shared" si="14"/>
+        <v>44813</v>
+      </c>
+      <c r="B51" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C51" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D51" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E51" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="10">
+        <v>47</v>
+      </c>
+      <c r="H51" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I51" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J51" s="8">
+        <f t="shared" ref="J51:J53" si="20">A51</f>
+        <v>44813</v>
+      </c>
+      <c r="K51" s="8">
+        <f t="shared" ref="K51:K65" si="21">J51+360</f>
+        <v>45173</v>
+      </c>
+      <c r="L51" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M51" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <f t="shared" si="14"/>
+        <v>44814</v>
+      </c>
+      <c r="B52" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C52" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D52" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E52" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H52" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I52" s="8">
+        <v>45908</v>
+      </c>
+      <c r="J52" s="8">
+        <f t="shared" si="20"/>
+        <v>44814</v>
+      </c>
+      <c r="K52" s="8">
+        <f t="shared" si="21"/>
+        <v>45174</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M52" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <f t="shared" si="14"/>
+        <v>44814</v>
+      </c>
+      <c r="B53" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C53" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D53" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E53" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" s="10">
+        <v>47</v>
+      </c>
+      <c r="H53" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I53" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J53" s="8">
+        <f t="shared" si="20"/>
+        <v>44814</v>
+      </c>
+      <c r="K53" s="8">
+        <f t="shared" si="21"/>
+        <v>45174</v>
+      </c>
+      <c r="L53" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M53" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <f t="shared" si="14"/>
+        <v>44815</v>
+      </c>
+      <c r="B54" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C54" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D54" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E54" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H54" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I54" s="8">
+        <f>A54</f>
+        <v>44815</v>
+      </c>
+      <c r="J54" s="8">
+        <f>A54</f>
+        <v>44815</v>
+      </c>
+      <c r="K54" s="8">
+        <f t="shared" si="21"/>
+        <v>45175</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M54" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <f t="shared" si="14"/>
+        <v>44815</v>
+      </c>
+      <c r="B55" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C55" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D55" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E55" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" s="10">
+        <v>47</v>
+      </c>
+      <c r="H55" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I55" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J55" s="8">
+        <f t="shared" ref="J55:J57" si="22">A55</f>
+        <v>44815</v>
+      </c>
+      <c r="K55" s="8">
+        <f t="shared" si="21"/>
+        <v>45175</v>
+      </c>
+      <c r="L55" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M55" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <f t="shared" si="14"/>
+        <v>44816</v>
+      </c>
+      <c r="B56" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C56" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D56" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H56" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I56" s="8">
+        <v>45908</v>
+      </c>
+      <c r="J56" s="8">
+        <f t="shared" si="22"/>
+        <v>44816</v>
+      </c>
+      <c r="K56" s="8">
+        <f t="shared" si="21"/>
+        <v>45176</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M56" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <f t="shared" si="14"/>
+        <v>44816</v>
+      </c>
+      <c r="B57" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C57" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D57" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E57" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="10">
+        <v>47</v>
+      </c>
+      <c r="H57" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I57" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J57" s="8">
+        <f t="shared" si="22"/>
+        <v>44816</v>
+      </c>
+      <c r="K57" s="8">
+        <f t="shared" si="21"/>
+        <v>45176</v>
+      </c>
+      <c r="L57" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M57" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <f t="shared" si="14"/>
+        <v>44817</v>
+      </c>
+      <c r="B58" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C58" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D58" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E58" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H58" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I58" s="8">
+        <f>A58</f>
+        <v>44817</v>
+      </c>
+      <c r="J58" s="8">
+        <f>A58</f>
+        <v>44817</v>
+      </c>
+      <c r="K58" s="8">
+        <f t="shared" si="21"/>
+        <v>45177</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M58" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <f t="shared" si="14"/>
+        <v>44817</v>
+      </c>
+      <c r="B59" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C59" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D59" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E59" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="10">
+        <v>47</v>
+      </c>
+      <c r="H59" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I59" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J59" s="8">
+        <f t="shared" ref="J59:J61" si="23">A59</f>
+        <v>44817</v>
+      </c>
+      <c r="K59" s="8">
+        <f t="shared" si="21"/>
+        <v>45177</v>
+      </c>
+      <c r="L59" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M59" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <f t="shared" si="14"/>
+        <v>44818</v>
+      </c>
+      <c r="B60" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C60" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D60" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E60" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H60" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I60" s="8">
+        <v>45908</v>
+      </c>
+      <c r="J60" s="8">
+        <f t="shared" si="23"/>
+        <v>44818</v>
+      </c>
+      <c r="K60" s="8">
+        <f t="shared" si="21"/>
+        <v>45178</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M60" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <f t="shared" si="14"/>
+        <v>44818</v>
+      </c>
+      <c r="B61" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C61" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D61" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E61" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="10">
+        <v>47</v>
+      </c>
+      <c r="H61" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I61" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J61" s="8">
+        <f t="shared" si="23"/>
+        <v>44818</v>
+      </c>
+      <c r="K61" s="8">
+        <f t="shared" si="21"/>
+        <v>45178</v>
+      </c>
+      <c r="L61" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M61" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <f t="shared" si="14"/>
+        <v>44819</v>
+      </c>
+      <c r="B62" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C62" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D62" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E62" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H62" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I62" s="8">
+        <f>A62</f>
+        <v>44819</v>
+      </c>
+      <c r="J62" s="8">
+        <f>A62</f>
+        <v>44819</v>
+      </c>
+      <c r="K62" s="8">
+        <f t="shared" si="21"/>
+        <v>45179</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M62" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <f t="shared" si="14"/>
+        <v>44819</v>
+      </c>
+      <c r="B63" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C63" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D63" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E63" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="10">
+        <v>47</v>
+      </c>
+      <c r="H63" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I63" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J63" s="8">
+        <f t="shared" ref="J63:J65" si="24">A63</f>
+        <v>44819</v>
+      </c>
+      <c r="K63" s="8">
+        <f t="shared" si="21"/>
+        <v>45179</v>
+      </c>
+      <c r="L63" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M63" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <f t="shared" si="14"/>
+        <v>44820</v>
+      </c>
+      <c r="B64" s="6">
+        <v>4444</v>
+      </c>
+      <c r="C64" s="6">
+        <v>123456</v>
+      </c>
+      <c r="D64" s="6">
+        <v>9001</v>
+      </c>
+      <c r="E64" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="H64" s="6">
+        <v>311001</v>
+      </c>
+      <c r="I64" s="8">
+        <v>45908</v>
+      </c>
+      <c r="J64" s="8">
+        <f t="shared" si="24"/>
+        <v>44820</v>
+      </c>
+      <c r="K64" s="8">
+        <f t="shared" si="21"/>
+        <v>45180</v>
+      </c>
+      <c r="L64" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M64" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <f t="shared" si="14"/>
+        <v>44820</v>
+      </c>
+      <c r="B65" s="10">
+        <v>4444</v>
+      </c>
+      <c r="C65" s="10">
+        <v>123456</v>
+      </c>
+      <c r="D65" s="10">
+        <v>9001</v>
+      </c>
+      <c r="E65" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="10">
+        <v>47</v>
+      </c>
+      <c r="H65" s="10">
+        <v>310030</v>
+      </c>
+      <c r="I65" s="12">
+        <v>45908</v>
+      </c>
+      <c r="J65" s="8">
+        <f t="shared" si="24"/>
+        <v>44820</v>
+      </c>
+      <c r="K65" s="8">
+        <f t="shared" si="21"/>
+        <v>45180</v>
+      </c>
+      <c r="L65" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M65" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>